<commit_message>
commit some demo test_case
</commit_message>
<xml_diff>
--- a/static/data/Delivery_System_V1.5.xlsx
+++ b/static/data/Delivery_System_V1.5.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Job\YL\codes\temp\yljk_test_api\static\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Common\Job\tmp\tmp_code\yl_test_api\static\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95815429-3EB7-4243-B354-65BF99359BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84917AA3-FDDA-468A-ABE8-AD7181BE71CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3863" yWindow="3863" windowWidth="16875" windowHeight="10634" tabRatio="878" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="878" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="登录模块" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2349" uniqueCount="933">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2349" uniqueCount="934">
   <si>
     <t>用例编号</t>
   </si>
@@ -4482,7 +4482,11 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>Loginxx003</t>
+    <t>Login001</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Login003</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -4895,23 +4899,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="10.1875" customWidth="1"/>
-    <col min="4" max="4" width="14.3125" customWidth="1"/>
-    <col min="5" max="5" width="29.6875" customWidth="1"/>
-    <col min="6" max="6" width="20.6875" customWidth="1"/>
-    <col min="7" max="7" width="32.6875" customWidth="1"/>
-    <col min="8" max="8" width="10.1875" customWidth="1"/>
+    <col min="3" max="3" width="10.25" customWidth="1"/>
+    <col min="4" max="4" width="14.375" customWidth="1"/>
+    <col min="5" max="5" width="29.75" customWidth="1"/>
+    <col min="6" max="6" width="20.75" customWidth="1"/>
+    <col min="7" max="7" width="32.75" customWidth="1"/>
+    <col min="8" max="8" width="10.25" customWidth="1"/>
     <col min="9" max="9" width="33" customWidth="1"/>
-    <col min="10" max="10" width="38.8125" customWidth="1"/>
-    <col min="11" max="11" width="22.6875" customWidth="1"/>
-    <col min="12" max="12" width="29.1875" customWidth="1"/>
+    <col min="10" max="10" width="38.875" customWidth="1"/>
+    <col min="11" max="11" width="22.75" customWidth="1"/>
+    <col min="12" max="12" width="29.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="3" customFormat="1">
@@ -4955,7 +4959,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="28.05" customHeight="1">
+    <row r="2" spans="1:13" ht="28.15" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>918</v>
       </c>
@@ -4997,8 +5001,8 @@
       </c>
     </row>
     <row r="3" spans="1:13" s="3" customFormat="1" ht="63" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>13</v>
+      <c r="A3" s="11" t="s">
+        <v>932</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>14</v>
@@ -5074,7 +5078,7 @@
     </row>
     <row r="5" spans="1:13" s="3" customFormat="1" ht="409.5">
       <c r="A5" s="11" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>14</v>
@@ -5130,7 +5134,7 @@
       <selection activeCell="A2" sqref="A2:IV2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
@@ -5173,7 +5177,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="28.05" customHeight="1">
+    <row r="2" spans="1:13" ht="28.15" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>918</v>
       </c>
@@ -5252,7 +5256,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="267.75">
+    <row r="4" spans="1:13" ht="242.25">
       <c r="A4" t="s">
         <v>718</v>
       </c>
@@ -5290,7 +5294,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="267.75">
+    <row r="5" spans="1:13" ht="242.25">
       <c r="A5" t="s">
         <v>724</v>
       </c>
@@ -5328,7 +5332,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="267.75">
+    <row r="6" spans="1:13" ht="242.25">
       <c r="A6" t="s">
         <v>728</v>
       </c>
@@ -5366,7 +5370,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="267.75">
+    <row r="7" spans="1:13" ht="242.25">
       <c r="A7" t="s">
         <v>734</v>
       </c>
@@ -5404,7 +5408,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="267.75">
+    <row r="8" spans="1:13" ht="242.25">
       <c r="A8" t="s">
         <v>740</v>
       </c>
@@ -5442,7 +5446,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="267.75">
+    <row r="9" spans="1:13" ht="242.25">
       <c r="A9" t="s">
         <v>746</v>
       </c>
@@ -5480,7 +5484,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="267.75">
+    <row r="10" spans="1:13" ht="242.25">
       <c r="A10" t="s">
         <v>752</v>
       </c>
@@ -5518,7 +5522,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="267.75">
+    <row r="11" spans="1:13" ht="242.25">
       <c r="A11" t="s">
         <v>754</v>
       </c>
@@ -5556,7 +5560,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="267.75">
+    <row r="12" spans="1:13" ht="242.25">
       <c r="A12" t="s">
         <v>756</v>
       </c>
@@ -5594,7 +5598,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="267.75">
+    <row r="13" spans="1:13" ht="242.25">
       <c r="A13" t="s">
         <v>763</v>
       </c>
@@ -5632,7 +5636,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="409.05" customHeight="1">
+    <row r="14" spans="1:13" ht="409.15" customHeight="1">
       <c r="A14" t="s">
         <v>769</v>
       </c>
@@ -5670,7 +5674,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="315">
+    <row r="15" spans="1:13" ht="285">
       <c r="A15" t="s">
         <v>776</v>
       </c>
@@ -5874,7 +5878,7 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
@@ -5917,7 +5921,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="28.05" customHeight="1">
+    <row r="2" spans="1:13" ht="28.15" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>918</v>
       </c>
@@ -5996,7 +6000,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="315">
+    <row r="4" spans="1:13" ht="285">
       <c r="A4" t="s">
         <v>805</v>
       </c>
@@ -6107,7 +6111,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="315">
+    <row r="7" spans="1:13" ht="285">
       <c r="A7" t="s">
         <v>821</v>
       </c>
@@ -6221,7 +6225,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="330.75">
+    <row r="10" spans="1:13" ht="299.25">
       <c r="A10" t="s">
         <v>837</v>
       </c>
@@ -6259,7 +6263,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="330.75">
+    <row r="11" spans="1:13" ht="299.25">
       <c r="A11" t="s">
         <v>842</v>
       </c>
@@ -6297,7 +6301,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="330.75">
+    <row r="12" spans="1:13" ht="299.25">
       <c r="A12" t="s">
         <v>848</v>
       </c>
@@ -6335,7 +6339,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="330.75">
+    <row r="13" spans="1:13" ht="299.25">
       <c r="A13" t="s">
         <v>855</v>
       </c>
@@ -6411,7 +6415,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="409.5">
+    <row r="15" spans="1:13" ht="370.5">
       <c r="A15" t="s">
         <v>866</v>
       </c>
@@ -6563,7 +6567,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="315">
+    <row r="19" spans="1:12" ht="285">
       <c r="A19" t="s">
         <v>884</v>
       </c>
@@ -6598,7 +6602,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="315">
+    <row r="20" spans="1:12" ht="285">
       <c r="A20" t="s">
         <v>887</v>
       </c>
@@ -6633,7 +6637,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="315">
+    <row r="21" spans="1:12" ht="285">
       <c r="A21" t="s">
         <v>892</v>
       </c>
@@ -6671,7 +6675,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="315">
+    <row r="22" spans="1:12" ht="285">
       <c r="A22" t="s">
         <v>897</v>
       </c>
@@ -6706,7 +6710,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="315">
+    <row r="23" spans="1:12" ht="285">
       <c r="A23" t="s">
         <v>901</v>
       </c>
@@ -6741,7 +6745,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="315">
+    <row r="24" spans="1:12" ht="285">
       <c r="A24" t="s">
         <v>905</v>
       </c>
@@ -6779,7 +6783,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="315">
+    <row r="25" spans="1:12" ht="285">
       <c r="A25" t="s">
         <v>911</v>
       </c>
@@ -6831,23 +6835,23 @@
       <selection activeCell="A2" sqref="A2:IV2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="38.8125" customWidth="1"/>
-    <col min="2" max="2" width="17.3125" customWidth="1"/>
+    <col min="1" max="1" width="38.875" customWidth="1"/>
+    <col min="2" max="2" width="17.375" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="7.6875" customWidth="1"/>
-    <col min="5" max="5" width="26.8125" customWidth="1"/>
-    <col min="6" max="6" width="22.3125" customWidth="1"/>
-    <col min="7" max="7" width="24.3125" customWidth="1"/>
-    <col min="8" max="8" width="9.8125" customWidth="1"/>
-    <col min="9" max="9" width="7.8125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="51.8125" customWidth="1"/>
+    <col min="4" max="4" width="7.75" customWidth="1"/>
+    <col min="5" max="5" width="26.875" customWidth="1"/>
+    <col min="6" max="6" width="22.375" customWidth="1"/>
+    <col min="7" max="7" width="24.375" customWidth="1"/>
+    <col min="8" max="8" width="9.875" customWidth="1"/>
+    <col min="9" max="9" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="51.875" customWidth="1"/>
     <col min="11" max="11" width="21" customWidth="1"/>
-    <col min="12" max="12" width="50.3125" customWidth="1"/>
+    <col min="12" max="12" width="50.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="28.05" customHeight="1">
+    <row r="1" spans="1:13" ht="28.15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6888,7 +6892,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="28.05" customHeight="1">
+    <row r="2" spans="1:13" ht="28.15" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>918</v>
       </c>
@@ -6929,7 +6933,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="256.14999999999998">
+    <row r="3" spans="1:13" ht="264">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -6967,7 +6971,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="256.14999999999998">
+    <row r="4" spans="1:13" ht="264">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -7005,7 +7009,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="283.5">
+    <row r="5" spans="1:13" ht="256.5">
       <c r="A5" s="10" t="s">
         <v>931</v>
       </c>
@@ -7043,7 +7047,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="409.5">
+    <row r="6" spans="1:13" ht="399">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -7081,7 +7085,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="409.5">
+    <row r="7" spans="1:13" ht="399">
       <c r="A7" t="s">
         <v>66</v>
       </c>
@@ -7119,7 +7123,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="47.25">
+    <row r="8" spans="1:13" ht="42.75">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -7154,7 +7158,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="47.25">
+    <row r="9" spans="1:13" ht="42.75">
       <c r="A9" t="s">
         <v>78</v>
       </c>
@@ -7189,7 +7193,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="47.25">
+    <row r="10" spans="1:13" ht="42.75">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -7227,7 +7231,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="47.25">
+    <row r="11" spans="1:13" ht="42.75">
       <c r="A11" t="s">
         <v>92</v>
       </c>
@@ -7338,7 +7342,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="378">
+    <row r="14" spans="1:13" ht="342">
       <c r="A14" t="s">
         <v>113</v>
       </c>
@@ -7452,7 +7456,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="94.5">
+    <row r="17" spans="1:12" ht="85.5">
       <c r="A17" t="s">
         <v>128</v>
       </c>
@@ -7490,7 +7494,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="393.75">
+    <row r="18" spans="1:12" ht="356.25">
       <c r="A18" t="s">
         <v>133</v>
       </c>
@@ -7566,7 +7570,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="63">
+    <row r="20" spans="1:12" ht="57">
       <c r="A20" t="s">
         <v>145</v>
       </c>
@@ -7601,7 +7605,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="63">
+    <row r="21" spans="1:12" ht="57">
       <c r="A21" t="s">
         <v>151</v>
       </c>
@@ -7636,7 +7640,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="63">
+    <row r="22" spans="1:12" ht="57">
       <c r="A22" t="s">
         <v>153</v>
       </c>
@@ -7671,7 +7675,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="110.25">
+    <row r="23" spans="1:12" ht="99.75">
       <c r="A23" t="s">
         <v>159</v>
       </c>
@@ -7709,7 +7713,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="110.25">
+    <row r="24" spans="1:12" ht="99.75">
       <c r="A24" t="s">
         <v>167</v>
       </c>
@@ -7747,7 +7751,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="220.5">
+    <row r="25" spans="1:12" ht="199.5">
       <c r="A25" t="s">
         <v>171</v>
       </c>
@@ -7785,7 +7789,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="141.75">
+    <row r="26" spans="1:12" ht="128.25">
       <c r="A26" t="s">
         <v>178</v>
       </c>
@@ -7823,7 +7827,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="63">
+    <row r="27" spans="1:12" ht="57">
       <c r="A27" t="s">
         <v>182</v>
       </c>
@@ -7858,7 +7862,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="63">
+    <row r="28" spans="1:12" ht="57">
       <c r="A28" t="s">
         <v>187</v>
       </c>
@@ -7893,7 +7897,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="47.25">
+    <row r="29" spans="1:12" ht="42.75">
       <c r="A29" t="s">
         <v>190</v>
       </c>
@@ -7928,7 +7932,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="47.25">
+    <row r="30" spans="1:12" ht="42.75">
       <c r="A30" t="s">
         <v>194</v>
       </c>
@@ -7966,7 +7970,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="47.25">
+    <row r="31" spans="1:12" ht="42.75">
       <c r="A31" t="s">
         <v>202</v>
       </c>
@@ -8004,7 +8008,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="47.25">
+    <row r="32" spans="1:12" ht="42.75">
       <c r="A32" t="s">
         <v>207</v>
       </c>
@@ -8039,7 +8043,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="63">
+    <row r="33" spans="1:12" ht="57">
       <c r="A33" t="s">
         <v>211</v>
       </c>
@@ -8077,7 +8081,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="252">
+    <row r="34" spans="1:12" ht="228">
       <c r="A34" t="s">
         <v>218</v>
       </c>
@@ -8115,7 +8119,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="63">
+    <row r="35" spans="1:12" ht="57">
       <c r="A35" t="s">
         <v>224</v>
       </c>
@@ -8153,7 +8157,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="63">
+    <row r="36" spans="1:12" ht="57">
       <c r="A36" t="s">
         <v>230</v>
       </c>
@@ -8191,7 +8195,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="63">
+    <row r="37" spans="1:12" ht="57">
       <c r="A37" t="s">
         <v>236</v>
       </c>
@@ -8226,7 +8230,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="94.5">
+    <row r="38" spans="1:12" ht="85.5">
       <c r="A38" t="s">
         <v>241</v>
       </c>
@@ -8264,7 +8268,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="252">
+    <row r="39" spans="1:12" ht="228">
       <c r="A39" t="s">
         <v>248</v>
       </c>
@@ -8302,7 +8306,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="63">
+    <row r="40" spans="1:12" ht="57">
       <c r="A40" t="s">
         <v>254</v>
       </c>
@@ -8340,7 +8344,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="47.25">
+    <row r="41" spans="1:12" ht="42.75">
       <c r="A41" t="s">
         <v>259</v>
       </c>
@@ -8372,7 +8376,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="63">
+    <row r="42" spans="1:12" ht="57">
       <c r="A42" t="s">
         <v>264</v>
       </c>
@@ -8404,7 +8408,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="94.5">
+    <row r="43" spans="1:12" ht="85.5">
       <c r="A43" t="s">
         <v>269</v>
       </c>
@@ -8442,7 +8446,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="252">
+    <row r="44" spans="1:12" ht="228">
       <c r="A44" t="s">
         <v>274</v>
       </c>
@@ -8480,7 +8484,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="63">
+    <row r="45" spans="1:12" ht="57">
       <c r="A45" t="s">
         <v>279</v>
       </c>
@@ -8518,7 +8522,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="94.5">
+    <row r="46" spans="1:12" ht="85.5">
       <c r="A46" t="s">
         <v>284</v>
       </c>
@@ -8556,7 +8560,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="252">
+    <row r="47" spans="1:12" ht="228">
       <c r="A47" t="s">
         <v>289</v>
       </c>
@@ -8594,7 +8598,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="47.25">
+    <row r="48" spans="1:12" ht="42.75">
       <c r="A48" t="s">
         <v>294</v>
       </c>
@@ -8632,7 +8636,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="110.25">
+    <row r="49" spans="1:12" ht="99.75">
       <c r="A49" t="s">
         <v>299</v>
       </c>
@@ -8670,7 +8674,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="63">
+    <row r="50" spans="1:12" ht="57">
       <c r="A50" t="s">
         <v>305</v>
       </c>
@@ -8708,7 +8712,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="78.75">
+    <row r="51" spans="1:12" ht="71.25">
       <c r="A51" t="s">
         <v>309</v>
       </c>
@@ -8746,7 +8750,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="78.75">
+    <row r="52" spans="1:12" ht="71.25">
       <c r="A52" t="s">
         <v>313</v>
       </c>
@@ -8784,7 +8788,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="78.75">
+    <row r="53" spans="1:12" ht="71.25">
       <c r="A53" t="s">
         <v>317</v>
       </c>
@@ -8822,7 +8826,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="78.75">
+    <row r="54" spans="1:12" ht="71.25">
       <c r="A54" t="s">
         <v>321</v>
       </c>
@@ -8860,7 +8864,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="94.5">
+    <row r="55" spans="1:12" ht="85.5">
       <c r="A55" t="s">
         <v>325</v>
       </c>
@@ -8898,7 +8902,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="94.5">
+    <row r="56" spans="1:12" ht="85.5">
       <c r="A56" t="s">
         <v>329</v>
       </c>
@@ -8936,7 +8940,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="78.75">
+    <row r="57" spans="1:12" ht="71.25">
       <c r="A57" t="s">
         <v>333</v>
       </c>
@@ -8974,7 +8978,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="63">
+    <row r="58" spans="1:12" ht="57">
       <c r="A58" t="s">
         <v>337</v>
       </c>
@@ -9027,9 +9031,9 @@
       <selection activeCell="A2" sqref="A2:IV2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="14.25"/>
   <cols>
-    <col min="12" max="12" width="39.8125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="39.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -9073,7 +9077,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="28.05" customHeight="1">
+    <row r="2" spans="1:13" ht="28.15" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>918</v>
       </c>
@@ -9164,19 +9168,19 @@
       <selection activeCell="A2" sqref="A2:IV2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="27.3125" customWidth="1"/>
-    <col min="2" max="2" width="20.8125" customWidth="1"/>
+    <col min="1" max="1" width="27.375" customWidth="1"/>
+    <col min="2" max="2" width="20.875" customWidth="1"/>
     <col min="3" max="3" width="21.5" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="24.3125" customWidth="1"/>
-    <col min="7" max="7" width="31.6875" customWidth="1"/>
+    <col min="6" max="6" width="24.375" customWidth="1"/>
+    <col min="7" max="7" width="31.75" customWidth="1"/>
     <col min="8" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="26.6875" customWidth="1"/>
-    <col min="11" max="11" width="15.3125" customWidth="1"/>
-    <col min="12" max="12" width="18.6875" customWidth="1"/>
+    <col min="10" max="10" width="26.75" customWidth="1"/>
+    <col min="11" max="11" width="15.375" customWidth="1"/>
+    <col min="12" max="12" width="18.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -9220,7 +9224,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="28.05" customHeight="1">
+    <row r="2" spans="1:13" ht="28.15" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>918</v>
       </c>
@@ -9261,7 +9265,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="157.5">
+    <row r="3" spans="1:13" ht="142.5">
       <c r="A3" s="3" t="s">
         <v>25</v>
       </c>
@@ -9300,7 +9304,7 @@
       </c>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" ht="58.15">
+    <row r="4" spans="1:13" ht="72">
       <c r="A4" s="3" t="s">
         <v>30</v>
       </c>
@@ -9339,7 +9343,7 @@
       </c>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:13" ht="47.25">
+    <row r="5" spans="1:13" ht="42.75">
       <c r="A5" t="s">
         <v>348</v>
       </c>
@@ -9450,7 +9454,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="204.75">
+    <row r="8" spans="1:13" ht="185.25">
       <c r="A8" t="s">
         <v>366</v>
       </c>
@@ -9488,7 +9492,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="204.75">
+    <row r="9" spans="1:13" ht="185.25">
       <c r="A9" t="s">
         <v>371</v>
       </c>
@@ -9523,7 +9527,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="204.75">
+    <row r="10" spans="1:13" ht="185.25">
       <c r="A10" t="s">
         <v>371</v>
       </c>
@@ -9558,7 +9562,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="204.75">
+    <row r="11" spans="1:13" ht="185.25">
       <c r="A11" s="3" t="s">
         <v>374</v>
       </c>
@@ -9593,7 +9597,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="204.75">
+    <row r="12" spans="1:13" ht="185.25">
       <c r="A12" s="3" t="s">
         <v>375</v>
       </c>
@@ -9992,7 +9996,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="141.75">
+    <row r="24" spans="1:12" ht="128.25">
       <c r="A24" t="s">
         <v>422</v>
       </c>
@@ -10030,7 +10034,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="141.75">
+    <row r="25" spans="1:12" ht="128.25">
       <c r="A25" t="s">
         <v>430</v>
       </c>
@@ -10068,7 +10072,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="141.75">
+    <row r="26" spans="1:12" ht="128.25">
       <c r="A26" t="s">
         <v>437</v>
       </c>
@@ -10106,7 +10110,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="267.75">
+    <row r="27" spans="1:12" ht="242.25">
       <c r="A27" t="s">
         <v>444</v>
       </c>
@@ -10158,20 +10162,20 @@
       <selection activeCell="A2" sqref="A2:IV2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="17.6875" customWidth="1"/>
-    <col min="2" max="2" width="13.1875" customWidth="1"/>
-    <col min="3" max="3" width="15.1875" customWidth="1"/>
+    <col min="1" max="1" width="17.75" customWidth="1"/>
+    <col min="2" max="2" width="13.25" customWidth="1"/>
+    <col min="3" max="3" width="15.25" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="18.1875" customWidth="1"/>
-    <col min="6" max="6" width="23.1875" customWidth="1"/>
-    <col min="7" max="7" width="18.3125" customWidth="1"/>
+    <col min="5" max="5" width="18.25" customWidth="1"/>
+    <col min="6" max="6" width="23.25" customWidth="1"/>
+    <col min="7" max="7" width="18.375" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
     <col min="9" max="9" width="6" customWidth="1"/>
-    <col min="10" max="10" width="28.1875" customWidth="1"/>
-    <col min="11" max="11" width="20.6875" customWidth="1"/>
-    <col min="12" max="12" width="43.6875" customWidth="1"/>
+    <col min="10" max="10" width="28.25" customWidth="1"/>
+    <col min="11" max="11" width="20.75" customWidth="1"/>
+    <col min="12" max="12" width="43.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -10215,7 +10219,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="28.05" customHeight="1">
+    <row r="2" spans="1:13" ht="28.15" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>918</v>
       </c>
@@ -10256,7 +10260,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="110.25">
+    <row r="3" spans="1:13" ht="99.75">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -10294,7 +10298,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="409.5">
+    <row r="4" spans="1:13" ht="399">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -10484,7 +10488,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="63">
+    <row r="9" spans="1:13" ht="57">
       <c r="A9" t="s">
         <v>482</v>
       </c>
@@ -10519,7 +10523,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="63">
+    <row r="10" spans="1:13" ht="57">
       <c r="A10" t="s">
         <v>486</v>
       </c>
@@ -10554,7 +10558,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="63">
+    <row r="11" spans="1:13" ht="57">
       <c r="A11" t="s">
         <v>489</v>
       </c>
@@ -10603,17 +10607,17 @@
       <selection activeCell="A2" sqref="A2:IV2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="35.3125" customWidth="1"/>
-    <col min="2" max="2" width="17.8125" customWidth="1"/>
+    <col min="1" max="1" width="35.375" customWidth="1"/>
+    <col min="2" max="2" width="17.875" customWidth="1"/>
     <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="5" max="5" width="20.1875" customWidth="1"/>
-    <col min="6" max="6" width="25.8125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="20.25" customWidth="1"/>
+    <col min="6" max="6" width="25.875" style="2" customWidth="1"/>
     <col min="7" max="7" width="28.5" customWidth="1"/>
-    <col min="10" max="10" width="21.1875" customWidth="1"/>
-    <col min="11" max="11" width="10.6875" customWidth="1"/>
-    <col min="12" max="12" width="17.3125" customWidth="1"/>
+    <col min="10" max="10" width="21.25" customWidth="1"/>
+    <col min="11" max="11" width="10.75" customWidth="1"/>
+    <col min="12" max="12" width="17.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -10657,7 +10661,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="28.05" customHeight="1">
+    <row r="2" spans="1:13" ht="28.15" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>918</v>
       </c>
@@ -10774,7 +10778,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="267.75">
+    <row r="5" spans="1:13" ht="242.25">
       <c r="A5" t="s">
         <v>508</v>
       </c>
@@ -10850,7 +10854,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="141.75">
+    <row r="7" spans="1:13" ht="128.25">
       <c r="A7" t="s">
         <v>520</v>
       </c>
@@ -10885,7 +10889,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="141.75">
+    <row r="8" spans="1:13" ht="128.25">
       <c r="A8" t="s">
         <v>522</v>
       </c>
@@ -10920,7 +10924,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="141.75">
+    <row r="9" spans="1:13" ht="128.25">
       <c r="A9" t="s">
         <v>524</v>
       </c>
@@ -10993,7 +10997,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="378">
+    <row r="11" spans="1:13" ht="342">
       <c r="A11" t="s">
         <v>533</v>
       </c>
@@ -11096,7 +11100,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="157.5">
+    <row r="14" spans="1:13" ht="142.5">
       <c r="A14" t="s">
         <v>543</v>
       </c>
@@ -11172,7 +11176,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="141.75">
+    <row r="16" spans="1:13" ht="128.25">
       <c r="A16" t="s">
         <v>553</v>
       </c>
@@ -11210,7 +11214,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="141.75">
+    <row r="17" spans="1:12" ht="128.25">
       <c r="A17" t="s">
         <v>558</v>
       </c>
@@ -11248,7 +11252,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="141.75">
+    <row r="18" spans="1:12" ht="128.25">
       <c r="A18" t="s">
         <v>561</v>
       </c>
@@ -11286,7 +11290,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="141.75">
+    <row r="19" spans="1:12" ht="128.25">
       <c r="A19" t="s">
         <v>430</v>
       </c>
@@ -11476,7 +11480,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="141.75">
+    <row r="24" spans="1:12" ht="128.25">
       <c r="A24" t="s">
         <v>593</v>
       </c>
@@ -11511,7 +11515,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="157.5">
+    <row r="25" spans="1:12" ht="142.5">
       <c r="A25" t="s">
         <v>600</v>
       </c>
@@ -11581,17 +11585,17 @@
       <selection activeCell="A2" sqref="A2:IV2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="3" width="17.8125" customWidth="1"/>
+    <col min="1" max="3" width="17.875" customWidth="1"/>
     <col min="4" max="4" width="6" customWidth="1"/>
-    <col min="5" max="5" width="9.6875" customWidth="1"/>
-    <col min="6" max="6" width="29.8125" customWidth="1"/>
-    <col min="7" max="7" width="26.1875" customWidth="1"/>
+    <col min="5" max="5" width="9.75" customWidth="1"/>
+    <col min="6" max="6" width="29.875" customWidth="1"/>
+    <col min="7" max="7" width="26.25" customWidth="1"/>
     <col min="8" max="9" width="11" customWidth="1"/>
     <col min="10" max="10" width="27" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="27.1875" customWidth="1"/>
+    <col min="12" max="12" width="27.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -11635,7 +11639,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="28.05" customHeight="1">
+    <row r="2" spans="1:13" ht="28.15" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>918</v>
       </c>
@@ -11728,18 +11732,18 @@
       <selection activeCell="A2" sqref="A2:IV2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="33.1875" customWidth="1"/>
-    <col min="2" max="2" width="16.3125" customWidth="1"/>
-    <col min="3" max="3" width="13.1875" customWidth="1"/>
+    <col min="1" max="1" width="33.25" customWidth="1"/>
+    <col min="2" max="2" width="16.375" customWidth="1"/>
+    <col min="3" max="3" width="13.25" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="23.3125" customWidth="1"/>
+    <col min="5" max="5" width="23.375" customWidth="1"/>
     <col min="6" max="6" width="25.5" customWidth="1"/>
     <col min="7" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="26.6875" customWidth="1"/>
+    <col min="10" max="10" width="26.75" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="27.1875" customWidth="1"/>
+    <col min="12" max="12" width="27.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -11783,7 +11787,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="28.05" customHeight="1">
+    <row r="2" spans="1:13" ht="28.15" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>918</v>
       </c>
@@ -11824,7 +11828,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="141.75">
+    <row r="3" spans="1:13" ht="128.25">
       <c r="A3" t="s">
         <v>610</v>
       </c>
@@ -11862,7 +11866,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="157.5">
+    <row r="4" spans="1:13" ht="142.5">
       <c r="A4" t="s">
         <v>618</v>
       </c>
@@ -11938,7 +11942,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="283.5">
+    <row r="6" spans="1:13" ht="256.5">
       <c r="A6" t="s">
         <v>626</v>
       </c>
@@ -11976,7 +11980,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="17" customHeight="1">
+    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1">
       <c r="A7" t="s">
         <v>630</v>
       </c>
@@ -12014,7 +12018,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="110.25">
+    <row r="8" spans="1:13" ht="99.75">
       <c r="A8" t="s">
         <v>636</v>
       </c>
@@ -12052,7 +12056,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="110.25">
+    <row r="9" spans="1:13" ht="99.75">
       <c r="A9" t="s">
         <v>640</v>
       </c>
@@ -12087,7 +12091,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="267.75">
+    <row r="10" spans="1:13" ht="242.25">
       <c r="A10" t="s">
         <v>644</v>
       </c>
@@ -12125,7 +12129,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="409.5">
+    <row r="11" spans="1:13" ht="384.75">
       <c r="A11" t="s">
         <v>651</v>
       </c>
@@ -12160,7 +12164,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="409.5">
+    <row r="12" spans="1:13" ht="384.75">
       <c r="A12" t="s">
         <v>655</v>
       </c>
@@ -12209,7 +12213,7 @@
       <selection activeCell="A2" sqref="A2:IV2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
@@ -12252,7 +12256,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="28.05" customHeight="1">
+    <row r="2" spans="1:13" ht="28.15" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>918</v>
       </c>
@@ -12442,7 +12446,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="220.5">
+    <row r="7" spans="1:13" ht="199.5">
       <c r="A7" t="s">
         <v>682</v>
       </c>
@@ -12480,7 +12484,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="220.5">
+    <row r="8" spans="1:13" ht="199.5">
       <c r="A8" t="s">
         <v>689</v>
       </c>
@@ -12518,7 +12522,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="204.75">
+    <row r="9" spans="1:13" ht="185.25">
       <c r="A9" t="s">
         <v>695</v>
       </c>
@@ -12556,7 +12560,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="204.75">
+    <row r="10" spans="1:13" ht="185.25">
       <c r="A10" t="s">
         <v>701</v>
       </c>
@@ -12594,7 +12598,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="189">
+    <row r="11" spans="1:13" ht="171">
       <c r="A11" t="s">
         <v>705</v>
       </c>

</xml_diff>